<commit_message>
atualização da aula 02 23
</commit_message>
<xml_diff>
--- a/UC12/_MiniProjeto/_BD/BD.xlsx
+++ b/UC12/_MiniProjeto/_BD/BD.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.lhjunior\source\repos\T13\UC12\_MiniProjeto\_BD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro.lhjunior\source\repos\T13\T13\UC12\_MiniProjeto\_BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F413873-27F8-44CA-88B7-05BB58DD5691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5037EA-665E-4D8F-9E34-4B8C5BFBD24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{654FF9CC-B08E-425B-AECF-702A2A1C74AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{654FF9CC-B08E-425B-AECF-702A2A1C74AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="75">
   <si>
     <t>Tabela</t>
   </si>
@@ -241,6 +242,27 @@
   </si>
   <si>
     <t>,</t>
+  </si>
+  <si>
+    <t>Insert into produto (</t>
+  </si>
+  <si>
+    <t>)values(</t>
+  </si>
+  <si>
+    <t>cboIDCategoria</t>
+  </si>
+  <si>
+    <t>txtValorCusto</t>
+  </si>
+  <si>
+    <t>txtValorVenda</t>
+  </si>
+  <si>
+    <t>txtOBS</t>
+  </si>
+  <si>
+    <t>cboStatus</t>
   </si>
 </sst>
 </file>
@@ -1563,8 +1585,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>123000</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="58" name="Tinta 57">
@@ -1583,7 +1605,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="58" name="Tinta 57">
@@ -1628,8 +1650,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>164040</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="61" name="Tinta 60">
@@ -1648,7 +1670,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="61" name="Tinta 60">
@@ -1693,8 +1715,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>186000</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="62" name="Tinta 61">
@@ -1713,7 +1735,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="62" name="Tinta 61">
@@ -1758,8 +1780,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>171600</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="65" name="Tinta 64">
@@ -1778,7 +1800,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="65" name="Tinta 64">
@@ -1823,8 +1845,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>152520</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="66" name="Tinta 65">
@@ -1843,7 +1865,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="66" name="Tinta 65">
@@ -1888,8 +1910,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>126600</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="70" name="Tinta 69">
@@ -1908,7 +1930,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="70" name="Tinta 69">
@@ -1953,8 +1975,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>15300</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="73" name="Tinta 72">
@@ -1973,7 +1995,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="73" name="Tinta 72">
@@ -2018,8 +2040,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>106800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="74" name="Tinta 73">
@@ -2038,7 +2060,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="74" name="Tinta 73">
@@ -2083,8 +2105,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>172680</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="78" name="Tinta 77">
@@ -2103,7 +2125,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="78" name="Tinta 77">
@@ -2148,8 +2170,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>178800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="85" name="Tinta 84">
@@ -2168,7 +2190,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="85" name="Tinta 84">
@@ -2213,8 +2235,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>74040</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="86" name="Tinta 85">
@@ -2233,7 +2255,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="86" name="Tinta 85">
@@ -2278,8 +2300,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>101040</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="93" name="Tinta 92">
@@ -2298,7 +2320,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="93" name="Tinta 92">
@@ -2343,8 +2365,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>133440</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="96" name="Tinta 95">
@@ -2363,7 +2385,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="96" name="Tinta 95">
@@ -2408,8 +2430,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>170580</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="97" name="Tinta 96">
@@ -2428,7 +2450,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="97" name="Tinta 96">
@@ -2473,8 +2495,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>174300</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="100" name="Tinta 99">
@@ -2493,7 +2515,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="100" name="Tinta 99">
@@ -2538,8 +2560,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>77760</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="101" name="Tinta 100">
@@ -2558,7 +2580,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="101" name="Tinta 100">
@@ -2603,8 +2625,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>38040</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="107" name="Tinta 106">
@@ -2623,7 +2645,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="107" name="Tinta 106">
@@ -2668,8 +2690,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>182520</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId35">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="108" name="Tinta 107">
@@ -2688,7 +2710,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="108" name="Tinta 107">
@@ -2733,8 +2755,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>28020</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId37">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="114" name="Tinta 113">
@@ -2753,7 +2775,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="114" name="Tinta 113">
@@ -2798,8 +2820,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>181800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId39">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="117" name="Tinta 116">
@@ -2818,7 +2840,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="117" name="Tinta 116">
@@ -2863,8 +2885,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>190380</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId41">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="118" name="Tinta 117">
@@ -2883,7 +2905,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="118" name="Tinta 117">
@@ -2928,8 +2950,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>181800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId43">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="122" name="Tinta 121">
@@ -2948,7 +2970,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="122" name="Tinta 121">
@@ -2993,8 +3015,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>36960</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId45">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="125" name="Tinta 124">
@@ -3013,7 +3035,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="125" name="Tinta 124">
@@ -3294,7 +3316,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">99 389 24575,'-5'0'0,"-5"5"0,-2 6 0,2 5 0,2 5 0,2 3 0,3 2 0,-3-3 0,-4-6 0,-2-1 0,3 1 0,1-2-8191</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2113.78">311 733 24575,'-3'-43'0,"-1"-1"0,-11-44 0,0 1 0,12 63 0,-4-18 0,3-1 0,1 0 0,3-50 0,0 92 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,0-1 0,13 12 0,16 45 0,-22-40 0,-5-10 0,16 31 0,2-2 0,1 0 0,2-2 0,1-1 0,56 57 0,-81-89 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,8-44 0,-8 31 0,10-61-119,7-41-504,4-156 0,-22 236-6203</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2113.77">311 733 24575,'-3'-43'0,"-1"-1"0,-11-44 0,0 1 0,12 63 0,-4-18 0,3-1 0,1 0 0,3-50 0,0 92 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,0-1 0,13 12 0,16 45 0,-22-40 0,-5-10 0,16 31 0,2-2 0,1 0 0,2-2 0,1-1 0,56 57 0,-81-89 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,8-44 0,-8 31 0,10-61-119,7-41-504,4-156 0,-22 236-6203</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -3518,7 +3540,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">32 238 24575,'0'-133'0,"-2"160"0,-1 1 0,-6 26 0,4-23 0,-3 43 0,9 175 0,-4-344 0,0 45 0,3 1 0,10-90 0,-9 134 0,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,1 0 0,-1 1 0,1-1 0,5-6 0,-7 10 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,2 1 0,9 13 0,0 0 0,-1 0 0,0 1 0,-1 0 0,-1 1 0,-1 0 0,0 1 0,5 18 0,4 7 0,16 35 0,27 60 0,-60-138 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,2-1 0,7-26 0,-3-42 0,-9-423-1365,3 467-5461</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1048.39">535 582 24575,'0'9'0,"-5"8"0,-6 1 0,-5 6 0,-5-1 0,-3 0 0,2 1 0,10-4 0,7-5-8191</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1048.38">535 582 24575,'0'9'0,"-5"8"0,-6 1 0,-5 6 0,-5-1 0,-3 0 0,2 1 0,10-4 0,7-5-8191</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -4004,8 +4026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{381D36B2-13C9-443E-A6FF-D850C2BCE733}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A18" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4648,4 +4670,180 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{794D2C3E-1EED-4C94-814F-14C4F34AFA9C}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="str">
+        <f>_xlfn.CONCAT(B1:B18)</f>
+        <v>Insert into produto (nome_Produto,id_categoria_Produto,valorcusto_Produto,valorvenda_Produto,descricao_Produto,qtde_Produto,obs_Produto,status_Produto)values('"+txtNome.Text+"','"+cboIDCategoria.Text+"','"+txtValorCusto.Text+"','"+txtValorVenda.Text+"','"+txtDescricao.Text+"','"+txtQtde.Text+"','"+txtOBS.Text+"','"+cboStatus.Text+"')"</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="str">
+        <f>A2&amp;","</f>
+        <v>nome_Produto,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B8" si="0">A3&amp;","</f>
+        <v>id_categoria_Produto,</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>valorcusto_Produto,</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>valorvenda_Produto,</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>descricao_Produto,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>qtde_Produto,</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>obs_Produto,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="str">
+        <f>A9</f>
+        <v>status_Produto</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="str">
+        <f>"'""+"&amp;A11&amp;".Text+""',"</f>
+        <v>'"+txtNome.Text+"',</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" ref="B12:B18" si="1">"'""+"&amp;A12&amp;".Text+""',"</f>
+        <v>'"+cboIDCategoria.Text+"',</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="1"/>
+        <v>'"+txtValorCusto.Text+"',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="1"/>
+        <v>'"+txtValorVenda.Text+"',</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="1"/>
+        <v>'"+txtDescricao.Text+"',</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="1"/>
+        <v>'"+txtQtde.Text+"',</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="1"/>
+        <v>'"+txtOBS.Text+"',</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="str">
+        <f>"'""+"&amp;A18&amp;".Text+""')"""</f>
+        <v>'"+cboStatus.Text+"')"</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>